<commit_message>
Creating a method that takes data from db and handles it in ExportToExcel
</commit_message>
<xml_diff>
--- a/aQord.ASP/Files/ExportToExcel/ProjectNummer_50518-Uge_19.xlsx
+++ b/aQord.ASP/Files/ExportToExcel/ProjectNummer_50518-Uge_19.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <x:si>
     <x:t xml:space="preserve">Arbejdets art: </x:t>
   </x:si>
@@ -119,6 +119,9 @@
   </x:si>
   <x:si>
     <x:t>Qu Le</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nicoline Kops Le</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> </x:t>
@@ -1555,87 +1558,189 @@
       <x:c r="V8" s="88" t="s"/>
     </x:row>
     <x:row r="9" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A9" s="89" t="s"/>
-      <x:c r="B9" s="89" t="s"/>
-      <x:c r="C9" s="79" t="s"/>
-      <x:c r="D9" s="89" t="s"/>
-      <x:c r="E9" s="89" t="s"/>
-      <x:c r="F9" s="89" t="s"/>
-      <x:c r="G9" s="89" t="s"/>
-      <x:c r="H9" s="89" t="s"/>
-      <x:c r="I9" s="89" t="s"/>
-      <x:c r="J9" s="89" t="s"/>
+      <x:c r="A9" s="89" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B9" s="89" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C9" s="79" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D9" s="89" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E9" s="89" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F9" s="89" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G9" s="89" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H9" s="89" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="I9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="K9" s="85">
         <x:f>SUM(D9:J9)</x:f>
       </x:c>
       <x:c r="L9" s="86" t="s"/>
-      <x:c r="M9" s="89" t="s"/>
-      <x:c r="N9" s="89" t="s"/>
-      <x:c r="O9" s="89" t="s"/>
-      <x:c r="P9" s="89" t="s"/>
-      <x:c r="Q9" s="89" t="s"/>
-      <x:c r="R9" s="89" t="s"/>
-      <x:c r="S9" s="89" t="s"/>
+      <x:c r="M9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="S9" s="89" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="T9" s="87">
         <x:f>SUM(M9:S9)</x:f>
       </x:c>
       <x:c r="U9" s="88" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V9" s="88" t="s"/>
     </x:row>
     <x:row r="10" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A10" s="90" t="s"/>
-      <x:c r="B10" s="90" t="s"/>
-      <x:c r="C10" s="79" t="s"/>
-      <x:c r="D10" s="90" t="s"/>
-      <x:c r="E10" s="90" t="s"/>
-      <x:c r="F10" s="90" t="s"/>
-      <x:c r="G10" s="90" t="s"/>
-      <x:c r="H10" s="90" t="s"/>
-      <x:c r="I10" s="90" t="s"/>
-      <x:c r="J10" s="90" t="s"/>
+      <x:c r="A10" s="90" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B10" s="90" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C10" s="79" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D10" s="90" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="90" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F10" s="90" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G10" s="90" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H10" s="90" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="I10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="K10" s="85">
         <x:f>SUM(D10:J10)</x:f>
       </x:c>
       <x:c r="L10" s="86" t="s"/>
-      <x:c r="M10" s="90" t="s"/>
-      <x:c r="N10" s="90" t="s"/>
-      <x:c r="O10" s="90" t="s"/>
-      <x:c r="P10" s="90" t="s"/>
-      <x:c r="Q10" s="90" t="s"/>
-      <x:c r="R10" s="90" t="s"/>
-      <x:c r="S10" s="90" t="s"/>
+      <x:c r="M10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="S10" s="90" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="T10" s="87">
         <x:f>SUM(M10:S10)</x:f>
       </x:c>
       <x:c r="U10" s="88" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="V10" s="88" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A11" s="91" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B11" s="83" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="V10" s="88" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A11" s="91" t="s"/>
-      <x:c r="B11" s="83" t="s"/>
-      <x:c r="C11" s="79" t="s"/>
-      <x:c r="D11" s="92" t="s"/>
-      <x:c r="E11" s="92" t="s"/>
-      <x:c r="F11" s="92" t="s"/>
-      <x:c r="G11" s="92" t="s"/>
-      <x:c r="H11" s="92" t="s"/>
-      <x:c r="I11" s="92" t="s"/>
-      <x:c r="J11" s="92" t="s"/>
+      <x:c r="C11" s="79" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D11" s="92" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E11" s="92" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F11" s="92" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G11" s="92" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H11" s="92" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="I11" s="92" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J11" s="92" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="K11" s="85">
         <x:f>SUM(D11:J11)</x:f>
       </x:c>
       <x:c r="L11" s="86" t="s"/>
-      <x:c r="M11" s="83" t="s"/>
-      <x:c r="N11" s="83" t="s"/>
-      <x:c r="O11" s="83" t="s"/>
-      <x:c r="P11" s="83" t="s"/>
-      <x:c r="Q11" s="83" t="s"/>
-      <x:c r="R11" s="83" t="s"/>
-      <x:c r="S11" s="83" t="s"/>
+      <x:c r="M11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="S11" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="T11" s="87">
         <x:f>SUM(M11:S11)</x:f>
       </x:c>
@@ -1836,7 +1941,7 @@
         <x:f>SUM(M18:S18)</x:f>
       </x:c>
       <x:c r="U18" s="88" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V18" s="88" t="s"/>
     </x:row>
@@ -1866,7 +1971,7 @@
         <x:f>SUM(M19:S19)</x:f>
       </x:c>
       <x:c r="U19" s="88" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V19" s="88" t="s"/>
     </x:row>
@@ -1944,7 +2049,7 @@
     </x:row>
     <x:row r="23" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="D23" s="58" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E23" s="98" t="s"/>
       <x:c r="F23" s="98" t="s"/>
@@ -1959,7 +2064,7 @@
         <x:f>SUM(L11:L22)</x:f>
       </x:c>
       <x:c r="M23" s="58" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="N23" s="98" t="s"/>
       <x:c r="O23" s="98" t="s"/>
@@ -1981,7 +2086,7 @@
     <x:row r="25" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="26" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A26" s="54" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B26" s="54" t="s"/>
       <x:c r="C26" s="54" t="s"/>
@@ -2001,7 +2106,7 @@
     <x:row r="27" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="28" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A28" s="54" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B28" s="54" t="s"/>
       <x:c r="C28" s="54" t="s"/>
@@ -3028,7 +3133,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A1" s="72" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="O1" s="3" t="s"/>
       <x:c r="P1" s="3" t="s"/>
@@ -3073,7 +3178,7 @@
     </x:row>
     <x:row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <x:c r="A3" s="73" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="O3" s="3" t="s"/>
       <x:c r="P3" s="3" t="s"/>
@@ -3119,12 +3224,12 @@
     <x:row r="5" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A5" s="3" t="s"/>
       <x:c r="B5" s="21" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G5" s="3" t="s"/>
       <x:c r="H5" s="3" t="s"/>
       <x:c r="I5" s="21" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="N5" s="3" t="s"/>
       <x:c r="O5" s="3" t="s"/>
@@ -3171,12 +3276,12 @@
     <x:row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <x:c r="A7" s="3" t="s"/>
       <x:c r="B7" s="73" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G7" s="3" t="s"/>
       <x:c r="H7" s="3" t="s"/>
       <x:c r="I7" s="73" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="N7" s="3" t="s"/>
       <x:c r="O7" s="3" t="s"/>
@@ -3194,7 +3299,7 @@
     </x:row>
     <x:row r="8" spans="1:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A8" s="25" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B8" s="26" t="s"/>
       <x:c r="C8" s="28" t="s"/>
@@ -3202,10 +3307,10 @@
       <x:c r="E8" s="28" t="s"/>
       <x:c r="F8" s="29" t="s"/>
       <x:c r="G8" s="25" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="H8" s="25" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="I8" s="26" t="s"/>
       <x:c r="J8" s="28" t="s"/>
@@ -3213,7 +3318,7 @@
       <x:c r="L8" s="28" t="s"/>
       <x:c r="M8" s="29" t="s"/>
       <x:c r="N8" s="25" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="O8" s="3" t="s"/>
       <x:c r="P8" s="3" t="s"/>

</xml_diff>

<commit_message>
ExportToExcel now works and is only exporting projectnumber with same weeknumber still need refactoring
</commit_message>
<xml_diff>
--- a/aQord.ASP/Files/ExportToExcel/ProjectNummer_50518-Uge_19.xlsx
+++ b/aQord.ASP/Files/ExportToExcel/ProjectNummer_50518-Uge_19.xlsx
@@ -1622,61 +1622,27 @@
       <x:c r="V9" s="88" t="s"/>
     </x:row>
     <x:row r="10" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A10" s="90" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B10" s="90" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C10" s="79" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D10" s="90" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E10" s="90" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F10" s="90" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="G10" s="90" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H10" s="90" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="I10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
+      <x:c r="A10" s="90" t="s"/>
+      <x:c r="B10" s="90" t="s"/>
+      <x:c r="C10" s="79" t="s"/>
+      <x:c r="D10" s="90" t="s"/>
+      <x:c r="E10" s="90" t="s"/>
+      <x:c r="F10" s="90" t="s"/>
+      <x:c r="G10" s="90" t="s"/>
+      <x:c r="H10" s="90" t="s"/>
+      <x:c r="I10" s="90" t="s"/>
+      <x:c r="J10" s="90" t="s"/>
       <x:c r="K10" s="85">
         <x:f>SUM(D10:J10)</x:f>
       </x:c>
       <x:c r="L10" s="86" t="s"/>
-      <x:c r="M10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="N10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="O10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="P10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="Q10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="R10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="S10" s="90" t="n">
-        <x:v>0</x:v>
-      </x:c>
+      <x:c r="M10" s="90" t="s"/>
+      <x:c r="N10" s="90" t="s"/>
+      <x:c r="O10" s="90" t="s"/>
+      <x:c r="P10" s="90" t="s"/>
+      <x:c r="Q10" s="90" t="s"/>
+      <x:c r="R10" s="90" t="s"/>
+      <x:c r="S10" s="90" t="s"/>
       <x:c r="T10" s="87">
         <x:f>SUM(M10:S10)</x:f>
       </x:c>
@@ -1686,61 +1652,27 @@
       <x:c r="V10" s="88" t="s"/>
     </x:row>
     <x:row r="11" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A11" s="91" t="n">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B11" s="83" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C11" s="79" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D11" s="92" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E11" s="92" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F11" s="92" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="G11" s="92" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="H11" s="92" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="I11" s="92" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J11" s="92" t="n">
-        <x:v>0</x:v>
-      </x:c>
+      <x:c r="A11" s="91" t="s"/>
+      <x:c r="B11" s="83" t="s"/>
+      <x:c r="C11" s="79" t="s"/>
+      <x:c r="D11" s="92" t="s"/>
+      <x:c r="E11" s="92" t="s"/>
+      <x:c r="F11" s="92" t="s"/>
+      <x:c r="G11" s="92" t="s"/>
+      <x:c r="H11" s="92" t="s"/>
+      <x:c r="I11" s="92" t="s"/>
+      <x:c r="J11" s="92" t="s"/>
       <x:c r="K11" s="85">
         <x:f>SUM(D11:J11)</x:f>
       </x:c>
       <x:c r="L11" s="86" t="s"/>
-      <x:c r="M11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="N11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="O11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="P11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="Q11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="R11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="S11" s="83" t="n">
-        <x:v>0</x:v>
-      </x:c>
+      <x:c r="M11" s="83" t="s"/>
+      <x:c r="N11" s="83" t="s"/>
+      <x:c r="O11" s="83" t="s"/>
+      <x:c r="P11" s="83" t="s"/>
+      <x:c r="Q11" s="83" t="s"/>
+      <x:c r="R11" s="83" t="s"/>
+      <x:c r="S11" s="83" t="s"/>
       <x:c r="T11" s="87">
         <x:f>SUM(M11:S11)</x:f>
       </x:c>

</xml_diff>